<commit_message>
re-created isotope data after excluding Switzerland
</commit_message>
<xml_diff>
--- a/data/Data_Aufwand_Nov2024.xlsx
+++ b/data/Data_Aufwand_Nov2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sop\OneDrive - Vogelwarte\Woodcock\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vogelwarte-my.sharepoint.com/personal/steffen_oppel_vogelwarte_ch/Documents/Woodcock/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C596CE96-94E6-4189-AE19-8DA36445566E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C596CE96-94E6-4189-AE19-8DA36445566E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60C7FBE0-BF27-40F2-965E-91FBB7328AD1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29AD3D1C-4ECC-462C-BDCB-4C65E2E21B22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{29AD3D1C-4ECC-462C-BDCB-4C65E2E21B22}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -444,18 +444,18 @@
   <dimension ref="A1:E283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42489</v>
       </c>
@@ -489,7 +489,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42492</v>
       </c>
@@ -506,7 +506,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>42493</v>
       </c>
@@ -523,7 +523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42494</v>
       </c>
@@ -540,7 +540,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>42495</v>
       </c>
@@ -557,7 +557,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>42496</v>
       </c>
@@ -574,7 +574,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>42497</v>
       </c>
@@ -591,7 +591,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>42498</v>
       </c>
@@ -608,7 +608,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>42499</v>
       </c>
@@ -625,7 +625,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>42500</v>
       </c>
@@ -642,7 +642,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>42505</v>
       </c>
@@ -659,7 +659,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>42507</v>
       </c>
@@ -676,7 +676,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>42509</v>
       </c>
@@ -693,7 +693,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>42510</v>
       </c>
@@ -710,7 +710,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>42511</v>
       </c>
@@ -727,7 +727,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>42514</v>
       </c>
@@ -744,7 +744,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>42528</v>
       </c>
@@ -761,7 +761,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>42515</v>
       </c>
@@ -778,7 +778,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>42530</v>
       </c>
@@ -795,7 +795,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>42531</v>
       </c>
@@ -812,7 +812,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>42533</v>
       </c>
@@ -829,7 +829,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>42535</v>
       </c>
@@ -846,7 +846,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>42541</v>
       </c>
@@ -863,7 +863,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>42542</v>
       </c>
@@ -880,7 +880,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>42543</v>
       </c>
@@ -897,7 +897,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>42543</v>
       </c>
@@ -914,7 +914,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>42544</v>
       </c>
@@ -931,7 +931,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>42545</v>
       </c>
@@ -948,7 +948,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>42545</v>
       </c>
@@ -965,7 +965,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>42546</v>
       </c>
@@ -982,7 +982,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>42548</v>
       </c>
@@ -999,7 +999,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>42549</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>42550</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>42550</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>42643</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>42558</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>42559</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>42560</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>42561</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>42565</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>42567</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42566</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>42569</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>42571</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>42571</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>42577</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>42577</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>42579</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>42579</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>42579</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>42583</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>42583</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>42584</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>42584</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>42585</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>42585</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>42585</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>42589</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>42589</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>42589</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>42590</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>42590</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>42590</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>42590</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>42590</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>42591</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>42591</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>42591</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>42591</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>42592</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>42593</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>42592</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>42592</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>42593</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>42593</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>42592</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>42593</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>42594</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>42594</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>42594</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>42597</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>42597</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>42597</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>42598</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>42598</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>42598</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>42599</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>42599</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>42601</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>42601</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>42604</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>42605</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>42605</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>42605</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>42606</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>42606</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>42607</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>42607</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>42608</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>42608</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>42608</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>42609</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>42610</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>42611</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>42611</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>42612</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>42612</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>42612</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>42613</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>42613</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>42634</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>42635</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>42635</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>42635</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>42614</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>42641</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>42641</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>42619</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>42621</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>42621</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>42816</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>42817</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>42818</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>42819</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>42821</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>42822</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>42823</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>42824</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>42825</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>42826</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>42828</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>42829</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>42830</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>42830</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>42831</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>42832</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>42837</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>42837</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>42838</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>42839</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>42844</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>42845</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>42846</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>42847</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>42848</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <v>42848</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>42849</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>42849</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>42850</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>42853</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>42854</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>42855</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>42855</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <v>42856</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>42859</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>42859</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>42860</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>42864</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>42864</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>42865</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <v>42865</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <v>42867</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <v>42877</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <v>42878</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>42879</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <v>42881</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>42881</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>42882</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <v>42883</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <v>42883</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>42884</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <v>42885</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>42887</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="2">
         <v>42888</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>42889</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <v>42890</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>42891</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>42892</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>42893</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>42898</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>42899</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>42899</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>42901</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>42902</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>42903</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>42906</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>42906</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>42906</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>42908</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>42909</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>42910</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="2">
         <v>42911</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>42912</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="2">
         <v>42912</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="2">
         <v>42912</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <v>42919</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>42920</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>42921</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>42922</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <v>42927</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>42928</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <v>42933</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>42934</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <v>42935</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <v>42941</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="2">
         <v>42942</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="2">
         <v>42943</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>42943</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <v>42949</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
         <v>42950</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="2">
         <v>42955</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="2">
         <v>42984</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <v>43195</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="2">
         <v>43196</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="2">
         <v>43200</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="2">
         <v>43200</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="2">
         <v>43201</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="2">
         <v>43202</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="2">
         <v>43206</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="2">
         <v>43207</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="2">
         <v>43207</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="2">
         <v>43208</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="2">
         <v>43208</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="2">
         <v>43209</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="2">
         <v>43209</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="2">
         <v>43210</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="2">
         <v>43213</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="2">
         <v>43214</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="2">
         <v>43215</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="2">
         <v>43216</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="2">
         <v>43238</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" s="2">
         <v>43242</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="2">
         <v>43243</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" s="2">
         <v>43244</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" s="2">
         <v>43246</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" s="2">
         <v>43246</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="2">
         <v>43245</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="2">
         <v>43249</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="2">
         <v>43250</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" s="2">
         <v>43252</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" s="2">
         <v>43253</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" s="2">
         <v>43256</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="2">
         <v>43258</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="2">
         <v>43264</v>
       </c>
@@ -4620,7 +4620,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" s="2">
         <v>43265</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="2">
         <v>43266</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="2">
         <v>43267</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="2">
         <v>43268</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="2">
         <v>43269</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="2">
         <v>43269</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" s="2">
         <v>43270</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="2">
         <v>43271</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="2">
         <v>43271</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="2">
         <v>43272</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" s="2">
         <v>43273</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" s="2">
         <v>43273</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" s="2">
         <v>43274</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" s="2">
         <v>43275</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="2">
         <v>43276</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" s="2">
         <v>43277</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" s="2">
         <v>43277</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" s="2">
         <v>43280</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" s="2">
         <v>43285</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" s="2">
         <v>43286</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" s="2">
         <v>43287</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" s="2">
         <v>43288</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" s="2">
         <v>43289</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" s="2">
         <v>43291</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" s="2">
         <v>43297</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" s="2">
         <v>43298</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" s="2">
         <v>43300</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" s="2">
         <v>43307</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" s="2">
         <v>43309</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" s="2">
         <v>43312</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" s="2">
         <v>43322</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" s="2">
         <v>43323</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" s="2">
         <v>43324</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" s="2">
         <v>43341</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" s="2">
         <v>43364</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" s="2">
         <v>43371</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" s="2">
         <v>43371</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" s="2">
         <v>43372</v>
       </c>
@@ -5267,7 +5267,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E121" xr:uid="{F29835B7-45FC-4D24-AD07-8A962B974640}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>